<commit_message>
Compare Swift-only data single and double resource
Former-commit-id: 939e065a97450da0cdff2a578dde8c4c96848c34
</commit_message>
<xml_diff>
--- a/Swift_Experiments/analysis/timings.xlsx
+++ b/Swift_Experiments/analysis/timings.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/SWIFT_exp/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33740" windowHeight="21700" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TTC_stampede" sheetId="1" r:id="rId1"/>
@@ -1194,6 +1194,544 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time to Completion (TTC) - Swift+Coaster</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Stampede</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TTC_stampede_gordon!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TTC_stampede!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>999.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1006.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1071.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7926.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Stampede, Gordon</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TTC_stampede_gordon!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TTC_stampede_gordon!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1107.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2860.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2848.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7659.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2070599920"/>
+        <c:axId val="-2071339248"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2070599920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2071339248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2071339248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2070599920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1274,6 +1812,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1778,6 +2356,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2339,6 +3420,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2784,7 +3897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2948,8 +4061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Plots and analysis data of Swift on single resource
</commit_message>
<xml_diff>
--- a/Swift_Experiments/analysis/timings.xlsx
+++ b/Swift_Experiments/analysis/timings.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,16 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TTC_stampede" sheetId="1" r:id="rId1"/>
     <sheet name="TTC_stampede_gordon" sheetId="2" r:id="rId2"/>
-    <sheet name="plots" sheetId="3" r:id="rId3"/>
+    <sheet name="Tw_stampede_gordon" sheetId="4" r:id="rId3"/>
+    <sheet name="Te_stampede_gordon" sheetId="5" r:id="rId4"/>
+    <sheet name="plots" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="TTC" localSheetId="0">TTC_stampede!$B$1:$E$7</definedName>
+    <definedName name="Executing_task" localSheetId="3">Te_stampede_gordon!$B$4:$E$7</definedName>
+    <definedName name="Queuing_block" localSheetId="2">Tw_stampede_gordon!$B$4:$E$7</definedName>
     <definedName name="TTC" localSheetId="1">TTC_stampede_gordon!$B$4:$E$7</definedName>
+    <definedName name="TTC_1" localSheetId="0">TTC_stampede!$B$4:$E$7</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,8 +35,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="TTC" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/SWIFT_exp/analysis/stampede/TTC.csv" comma="1">
+  <connection id="1" name="Executing_task" type="6" refreshedVersion="0" deleted="1" background="1" saveData="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/analysis/stampede_gordon/Executing_task.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -41,8 +45,28 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="TTC1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/SWIFT_exp/analysis/stampede_gordon/TTC.csv" comma="1">
+  <connection id="2" name="Queuing_block" type="6" refreshedVersion="0" deleted="1" background="1" saveData="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/analysis/stampede_gordon/Submitting_task.csv" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="TTC" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/analysis/stampede/TTC.csv" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="TTC1" type="6" refreshedVersion="0" deleted="1" background="1" saveData="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/analysis/stampede_gordon/TTC.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -55,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
   <si>
     <t>AVG</t>
   </si>
@@ -375,18 +399,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>256.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2048.0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -423,11 +435,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2120829472"/>
-        <c:axId val="-2120821328"/>
+        <c:axId val="-2080530336"/>
+        <c:axId val="-2080522960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2120829472"/>
+        <c:axId val="-2080530336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +538,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120821328"/>
+        <c:crossAx val="-2080522960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -534,7 +546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2120821328"/>
+        <c:axId val="-2080522960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,7 +658,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120829472"/>
+        <c:crossAx val="-2080530336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -729,7 +741,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" b="1"/>
               <a:t>Time to Completion (TTC) - Swift+Coaster</a:t>
             </a:r>
           </a:p>
@@ -739,7 +751,33 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Stampede</a:t>
+              <a:t>Stampede and Gordon</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Includes: Setup, queuing, bootstrapping, stage in, execution, stage out, shutdown times</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Queuing time accounts for</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> the majority of the timing and of the variation.</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -789,7 +827,7 @@
           <c:spPr>
             <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -922,11 +960,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2079178496"/>
-        <c:axId val="-2079177488"/>
+        <c:axId val="-2080418928"/>
+        <c:axId val="-2080413024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2079178496"/>
+        <c:axId val="-2080418928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,7 +1063,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079177488"/>
+        <c:crossAx val="-2080413024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1033,7 +1071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2079177488"/>
+        <c:axId val="-2080413024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,7 +1183,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079178496"/>
+        <c:crossAx val="-2080418928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1353,7 +1391,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1428,11 +1466,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2070599920"/>
-        <c:axId val="-2071339248"/>
+        <c:axId val="-2082600880"/>
+        <c:axId val="-2082595264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2070599920"/>
+        <c:axId val="-2082600880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1531,7 +1569,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071339248"/>
+        <c:crossAx val="-2082595264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1539,7 +1577,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2071339248"/>
+        <c:axId val="-2082595264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12000.0"/>
@@ -1652,7 +1690,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2070599920"/>
+        <c:crossAx val="-2082600880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1696,6 +1734,1052 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Waiting Time (Tw) - Swift+Coaster</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Stampede and Gordon</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Includes: setup</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>, queueing , and bootstrapping times. </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Queuing time accounts for the majority of the timing and of the variation.  </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Tw</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Tw_stampede_gordon!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>42.99297423223163</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1837.680739410412</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1707.512054618258</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2570.537990868837</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Tw_stampede_gordon!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>42.99297423223163</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1837.680739410412</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1707.512054618258</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2570.537990868837</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tw_stampede_gordon!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tw_stampede_gordon!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>205.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1958.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1947.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6754.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2037913984"/>
+        <c:axId val="-2030674128"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2037913984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2030674128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2030674128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="12000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2037913984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Execution Time (Te) - Swift+Coaster</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Stampede and Gordon</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Includes: stage</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> in, executing , and stage out times. </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Very little variation, when present due to issues with staging out of err/out files.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Te</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Te_stampede_gordon!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>41.12253032098097</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>19.86359735798126</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>36.29279083601407</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1026.074670365986</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Te_stampede_gordon!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>41.12253032098097</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>19.86359735798126</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>36.29279083601407</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1026.074670365986</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>Te_stampede_gordon!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Te_stampede_gordon!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1057.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>959.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1059.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4048.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-1987154864"/>
+        <c:axId val="-2071059360"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1987154864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2071059360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2071059360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="12000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1987154864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1853,6 +2937,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2860,6 +4024,1012 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3458,15 +5628,87 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Queuing_block" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Executing_task" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3735,29 +5977,23 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="3" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="1">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1">
-        <v>32</v>
-      </c>
-      <c r="D1" s="1">
-        <v>256</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2048</v>
-      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -3767,15 +6003,15 @@
         <f>AVERAGE(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))</f>
         <v>999</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <f>AVERAGE(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))</f>
         <v>1006.5</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <f>AVERAGE(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))</f>
         <v>1071</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <f>AVERAGE(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))</f>
         <v>7926</v>
       </c>
@@ -3898,8 +6134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4060,10 +6296,340 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="4.1640625" customWidth="1"/>
+    <col min="3" max="4" width="5.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="1">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1">
+        <v>256</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <f>AVERAGE(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))</f>
+        <v>205.75</v>
+      </c>
+      <c r="C2" s="6">
+        <f>AVERAGE(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))</f>
+        <v>1958</v>
+      </c>
+      <c r="D2" s="6">
+        <f>AVERAGE(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))</f>
+        <v>1947.5</v>
+      </c>
+      <c r="E2" s="6">
+        <f>AVERAGE(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))</f>
+        <v>6754.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f>_xlfn.STDEV.S(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))/SQRT(COUNT(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26))))</f>
+        <v>42.992974232231632</v>
+      </c>
+      <c r="C3" s="2">
+        <f>_xlfn.STDEV.S(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))/SQRT(COUNT(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26))))</f>
+        <v>1837.6807394104123</v>
+      </c>
+      <c r="D3" s="2">
+        <f>_xlfn.STDEV.S(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))/SQRT(COUNT(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26))))</f>
+        <v>1707.5120546182584</v>
+      </c>
+      <c r="E3" s="2">
+        <f>_xlfn.STDEV.S(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))/SQRT(COUNT(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26))))</f>
+        <v>2570.5379908688374</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>216</v>
+      </c>
+      <c r="C4">
+        <v>7471</v>
+      </c>
+      <c r="D4">
+        <v>7070</v>
+      </c>
+      <c r="E4">
+        <v>14446</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>323</v>
+      </c>
+      <c r="C5">
+        <v>139</v>
+      </c>
+      <c r="D5">
+        <v>257</v>
+      </c>
+      <c r="E5">
+        <v>4718</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>132</v>
+      </c>
+      <c r="C6">
+        <v>118</v>
+      </c>
+      <c r="D6">
+        <v>226</v>
+      </c>
+      <c r="E6">
+        <v>3956</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>152</v>
+      </c>
+      <c r="C7">
+        <v>104</v>
+      </c>
+      <c r="D7">
+        <v>237</v>
+      </c>
+      <c r="E7">
+        <v>3899</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="3" max="3" width="4.1640625" customWidth="1"/>
+    <col min="4" max="5" width="5.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="1">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1">
+        <v>256</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <f>AVERAGE(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))</f>
+        <v>1057.75</v>
+      </c>
+      <c r="C2" s="6">
+        <f>AVERAGE(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))</f>
+        <v>959.75</v>
+      </c>
+      <c r="D2" s="6">
+        <f>AVERAGE(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))</f>
+        <v>1059</v>
+      </c>
+      <c r="E2" s="6">
+        <f>AVERAGE(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))</f>
+        <v>4048.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f>_xlfn.STDEV.S(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))/SQRT(COUNT(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26))))</f>
+        <v>41.122530320980978</v>
+      </c>
+      <c r="C3" s="2">
+        <f>_xlfn.STDEV.S(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))/SQRT(COUNT(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26))))</f>
+        <v>19.863597357981259</v>
+      </c>
+      <c r="D3" s="2">
+        <f>_xlfn.STDEV.S(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))/SQRT(COUNT(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26))))</f>
+        <v>36.292790836014071</v>
+      </c>
+      <c r="E3" s="2">
+        <f>_xlfn.STDEV.S(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))/SQRT(COUNT(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26))))</f>
+        <v>1026.0746703659859</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1058</v>
+      </c>
+      <c r="C4">
+        <v>901</v>
+      </c>
+      <c r="D4">
+        <v>954</v>
+      </c>
+      <c r="E4">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1172</v>
+      </c>
+      <c r="C5">
+        <v>985</v>
+      </c>
+      <c r="D5">
+        <v>1105</v>
+      </c>
+      <c r="E5">
+        <v>5582</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>982</v>
+      </c>
+      <c r="C6">
+        <v>983</v>
+      </c>
+      <c r="D6">
+        <v>1067</v>
+      </c>
+      <c r="E6">
+        <v>4827</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1019</v>
+      </c>
+      <c r="C7">
+        <v>970</v>
+      </c>
+      <c r="D7">
+        <v>1110</v>
+      </c>
+      <c r="E7">
+        <v>4763</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Onging refactoring of timings to calculate range overlapping in multi-host experiments
</commit_message>
<xml_diff>
--- a/Swift_Experiments/analysis/timings.xlsx
+++ b/Swift_Experiments/analysis/timings.xlsx
@@ -9,19 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TTC_stampede" sheetId="1" r:id="rId1"/>
-    <sheet name="TTC_stampede_gordon" sheetId="2" r:id="rId2"/>
-    <sheet name="Tw_stampede_gordon" sheetId="4" r:id="rId3"/>
-    <sheet name="Te_stampede_gordon" sheetId="5" r:id="rId4"/>
-    <sheet name="plots" sheetId="3" r:id="rId5"/>
+    <sheet name="Tw_stampede" sheetId="6" r:id="rId2"/>
+    <sheet name="Te_stampede" sheetId="7" r:id="rId3"/>
+    <sheet name="TTC_stampede_gordon" sheetId="2" r:id="rId4"/>
+    <sheet name="Tw_stampede_gordon" sheetId="4" r:id="rId5"/>
+    <sheet name="Te_stampede_gordon" sheetId="5" r:id="rId6"/>
+    <sheet name="plots" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="Executing_task" localSheetId="3">Te_stampede_gordon!$B$4:$E$7</definedName>
-    <definedName name="Queuing_block" localSheetId="2">Tw_stampede_gordon!$B$4:$E$7</definedName>
-    <definedName name="TTC" localSheetId="1">TTC_stampede_gordon!$B$4:$E$7</definedName>
+    <definedName name="Executing_task" localSheetId="2">Te_stampede!$B$4:$E$7</definedName>
+    <definedName name="Executing_task" localSheetId="5">Te_stampede_gordon!$B$4:$E$7</definedName>
+    <definedName name="Queuing_block" localSheetId="4">Tw_stampede_gordon!$B$4:$E$7</definedName>
+    <definedName name="Submitting_task" localSheetId="1">Tw_stampede!$B$4:$E$7</definedName>
+    <definedName name="TTC" localSheetId="3">TTC_stampede_gordon!$B$4:$E$7</definedName>
     <definedName name="TTC_1" localSheetId="0">TTC_stampede!$B$4:$E$7</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -35,8 +39,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Executing_task" type="6" refreshedVersion="0" deleted="1" background="1" saveData="1">
-    <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/analysis/stampede_gordon/Executing_task.csv" comma="1">
+  <connection id="1" name="Executing_task" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/analysis/stampede/Executing_task.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -55,8 +59,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="TTC" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/analysis/stampede/TTC.csv" comma="1">
+  <connection id="3" name="Submitting_task" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/analysis/stampede/Submitting_task.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -65,8 +69,18 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="TTC1" type="6" refreshedVersion="0" deleted="1" background="1" saveData="1">
-    <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/analysis/stampede_gordon/TTC.csv" comma="1">
+  <connection id="4" name="TTC" type="6" refreshedVersion="0" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/analysis/stampede/TTC.csv" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="TTC1" type="6" refreshedVersion="0" deleted="1" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" fileType="mac" codePage="10000" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/analysis/stampede/TTC.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -79,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="10">
   <si>
     <t>AVG</t>
   </si>
@@ -240,13 +254,27 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  </a:sysClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -254,18 +282,110 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1400" b="1"/>
               <a:t>Time to Completion (TTC) - Swift+Coaster</a:t>
             </a:r>
           </a:p>
           <a:p>
-            <a:pPr>
-              <a:defRPr/>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1400"/>
               <a:t>Stampede</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Includes: Setup, queuing, bootstrapping, stage in, execution, stage out, shutdown times</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1400"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -282,13 +402,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -399,6 +533,18 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -549,6 +695,7 @@
         <c:axId val="-2080522960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="12000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2817,6 +2964,1259 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1"/>
+              <a:t>Waiting Time (Tw) - Swift+Coaster</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Stampede</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Includes: </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>setup, queueing , and bootstrapping times.</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Variation</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> shows anomalously uniform queuing times. More runs should increase variation.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>TTC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Tw_stampede!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>7.756717518813397</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.685557397915996</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>17.40210715210469</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>46.57856266567271</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Tw_stampede!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>7.756717518813397</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.685557397915996</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>17.40210715210469</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>46.57856266567271</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>TTC_stampede!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TTC_stampede!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>999.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1006.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1071.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7926.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2036249536"/>
+        <c:axId val="-2036137312"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2036249536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2036137312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2036137312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="12000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2036249536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1"/>
+              <a:t>Execution Time (Te) - Swift+Coaster</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Stampede</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Includes: </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>: stage in, executing , and stage out times.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>No error bars, equal execution time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> as expected on same machine and same n of blocks.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Te</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Te_stampede!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.288675134594813</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.428133714055577</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>16.90414150437697</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>11.17661248619932</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Te_stampede!$B$3:$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.288675134594813</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.428133714055577</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>16.90414150437697</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>11.17661248619932</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>Te_stampede!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Te_stampede!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>900.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>903.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>975.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>987.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2013608032"/>
+        <c:axId val="-1987305104"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2013608032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1987305104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1987305104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="12000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2013608032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3017,6 +4417,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -5030,6 +6510,1012 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5692,22 +8178,94 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC_1" refreshOnLoad="1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Submitting_task" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Executing_task" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC" refreshOnLoad="1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Queuing_block" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Executing_task" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -5977,7 +8535,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5990,10 +8548,18 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="1">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1">
+        <v>256</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2048</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -6134,8 +8700,338 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="4.1640625" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="1">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1">
+        <v>256</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <f>AVERAGE(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))</f>
+        <v>97</v>
+      </c>
+      <c r="C2" s="5">
+        <f>AVERAGE(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))</f>
+        <v>105.5</v>
+      </c>
+      <c r="D2" s="5">
+        <f>AVERAGE(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))</f>
+        <v>169</v>
+      </c>
+      <c r="E2" s="5">
+        <f>AVERAGE(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))</f>
+        <v>7024.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f>_xlfn.STDEV.S(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))/SQRT(COUNT(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26))))</f>
+        <v>7.7567175188133968</v>
+      </c>
+      <c r="C3" s="2">
+        <f>_xlfn.STDEV.S(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))/SQRT(COUNT(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26))))</f>
+        <v>3.6855573979159968</v>
+      </c>
+      <c r="D3" s="2">
+        <f>_xlfn.STDEV.S(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))/SQRT(COUNT(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26))))</f>
+        <v>17.402107152104694</v>
+      </c>
+      <c r="E3" s="2">
+        <f>_xlfn.STDEV.S(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))/SQRT(COUNT(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26))))</f>
+        <v>46.578562665672713</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>91</v>
+      </c>
+      <c r="C4">
+        <v>105</v>
+      </c>
+      <c r="D4">
+        <v>143</v>
+      </c>
+      <c r="E4">
+        <v>6952</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>86</v>
+      </c>
+      <c r="C5">
+        <v>97</v>
+      </c>
+      <c r="D5">
+        <v>135</v>
+      </c>
+      <c r="E5">
+        <v>6984</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>120</v>
+      </c>
+      <c r="C6">
+        <v>115</v>
+      </c>
+      <c r="D6">
+        <v>200</v>
+      </c>
+      <c r="E6">
+        <v>7161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>91</v>
+      </c>
+      <c r="C7">
+        <v>105</v>
+      </c>
+      <c r="D7">
+        <v>198</v>
+      </c>
+      <c r="E7">
+        <v>7002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4.1640625" customWidth="1"/>
+    <col min="4" max="5" width="5.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="1">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1">
+        <v>256</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <f>AVERAGE(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))</f>
+        <v>900.5</v>
+      </c>
+      <c r="C2" s="5">
+        <f>AVERAGE(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))</f>
+        <v>903.75</v>
+      </c>
+      <c r="D2" s="5">
+        <f>AVERAGE(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))</f>
+        <v>975.5</v>
+      </c>
+      <c r="E2" s="5">
+        <f>AVERAGE(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))</f>
+        <v>987.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f>_xlfn.STDEV.S(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))/SQRT(COUNT(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26))))</f>
+        <v>0.28867513459481287</v>
+      </c>
+      <c r="C3" s="2">
+        <f>_xlfn.STDEV.S(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))/SQRT(COUNT(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26))))</f>
+        <v>2.4281337140555777</v>
+      </c>
+      <c r="D3" s="2">
+        <f>_xlfn.STDEV.S(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))/SQRT(COUNT(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26))))</f>
+        <v>16.904141504376966</v>
+      </c>
+      <c r="E3" s="2">
+        <f>_xlfn.STDEV.S(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))/SQRT(COUNT(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26))))</f>
+        <v>11.176612486199325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>901</v>
+      </c>
+      <c r="C4">
+        <v>902</v>
+      </c>
+      <c r="D4">
+        <v>952</v>
+      </c>
+      <c r="E4">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>901</v>
+      </c>
+      <c r="C5">
+        <v>901</v>
+      </c>
+      <c r="D5">
+        <v>941</v>
+      </c>
+      <c r="E5">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>900</v>
+      </c>
+      <c r="C6">
+        <v>901</v>
+      </c>
+      <c r="D6">
+        <v>1003</v>
+      </c>
+      <c r="E6">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>900</v>
+      </c>
+      <c r="C7">
+        <v>911</v>
+      </c>
+      <c r="D7">
+        <v>1006</v>
+      </c>
+      <c r="E7">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6294,7 +9190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -6459,7 +9355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -6624,12 +9520,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>